<commit_message>
Add Loader for Course Table
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="138">
   <si>
     <t>Teacher Name</t>
   </si>
@@ -362,6 +362,72 @@
   </si>
   <si>
     <t>CS6</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>test9</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>test15</t>
+  </si>
+  <si>
+    <t>test16</t>
+  </si>
+  <si>
+    <t>test17</t>
+  </si>
+  <si>
+    <t>test18</t>
+  </si>
+  <si>
+    <t>test19</t>
+  </si>
+  <si>
+    <t>test20</t>
+  </si>
+  <si>
+    <t>test21</t>
+  </si>
+  <si>
+    <t>test22</t>
   </si>
 </sst>
 </file>
@@ -756,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
@@ -992,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1002,8 +1068,11 @@
       <c r="C17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1013,8 +1082,11 @@
       <c r="C18" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1024,8 +1096,11 @@
       <c r="C19" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1035,8 +1110,11 @@
       <c r="C20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1046,8 +1124,11 @@
       <c r="C21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1057,8 +1138,11 @@
       <c r="C22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1068,8 +1152,11 @@
       <c r="C23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1079,8 +1166,11 @@
       <c r="C24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1090,8 +1180,11 @@
       <c r="C25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1101,8 +1194,11 @@
       <c r="C26" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1112,8 +1208,11 @@
       <c r="C27" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -1123,8 +1222,11 @@
       <c r="C28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1134,8 +1236,11 @@
       <c r="C29" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1145,8 +1250,11 @@
       <c r="C30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1156,8 +1264,11 @@
       <c r="C31" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -1167,8 +1278,11 @@
       <c r="C32" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1178,8 +1292,11 @@
       <c r="C33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1189,8 +1306,11 @@
       <c r="C34" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1200,8 +1320,11 @@
       <c r="C35" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1211,8 +1334,11 @@
       <c r="C36" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1222,8 +1348,11 @@
       <c r="C37" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1233,8 +1362,11 @@
       <c r="C38" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1244,8 +1376,11 @@
       <c r="C39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1255,8 +1390,11 @@
       <c r="C40" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1266,8 +1404,11 @@
       <c r="C41" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1277,8 +1418,11 @@
       <c r="C42" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1288,8 +1432,11 @@
       <c r="C43" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1299,8 +1446,11 @@
       <c r="C44" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1310,8 +1460,11 @@
       <c r="C45" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -1321,8 +1474,11 @@
       <c r="C46" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -1332,8 +1488,11 @@
       <c r="C47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1343,8 +1502,11 @@
       <c r="C48" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -1354,8 +1516,11 @@
       <c r="C49" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1365,8 +1530,11 @@
       <c r="C50" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -1376,8 +1544,11 @@
       <c r="C51" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -1387,8 +1558,11 @@
       <c r="C52" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1398,8 +1572,11 @@
       <c r="C53" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -1409,8 +1586,11 @@
       <c r="C54" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -1420,8 +1600,11 @@
       <c r="C55" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1431,8 +1614,11 @@
       <c r="C56" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -1442,8 +1628,11 @@
       <c r="C57" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>50</v>
       </c>
@@ -1452,6 +1641,9 @@
       </c>
       <c r="C58" t="s">
         <v>115</v>
+      </c>
+      <c r="D58" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add RoomNo String to CourseTimesList
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -34,18 +34,9 @@
     <t>Naveera Sami</t>
   </si>
   <si>
-    <t>CS101-LA1</t>
-  </si>
-  <si>
     <t>Munazza Kanwal</t>
   </si>
   <si>
-    <t>CS102-LA2</t>
-  </si>
-  <si>
-    <t>CS102-LA1</t>
-  </si>
-  <si>
     <t>CS101A</t>
   </si>
   <si>
@@ -61,36 +52,6 @@
     <t>CS102B</t>
   </si>
   <si>
-    <t>CS102-LB1</t>
-  </si>
-  <si>
-    <t>CS102-LB2</t>
-  </si>
-  <si>
-    <t>CS101-LA2</t>
-  </si>
-  <si>
-    <t>CS101-LB</t>
-  </si>
-  <si>
-    <t>CS103-LA</t>
-  </si>
-  <si>
-    <t>NS104-LA</t>
-  </si>
-  <si>
-    <t>CS104-LA</t>
-  </si>
-  <si>
-    <t>NS104-LB</t>
-  </si>
-  <si>
-    <t>CS103-LB</t>
-  </si>
-  <si>
-    <t>CS104-LB</t>
-  </si>
-  <si>
     <t>CS201</t>
   </si>
   <si>
@@ -428,6 +389,45 @@
   </si>
   <si>
     <t>test22</t>
+  </si>
+  <si>
+    <t>CS102A-L1</t>
+  </si>
+  <si>
+    <t>CS102A-L2</t>
+  </si>
+  <si>
+    <t>CS102B-L1</t>
+  </si>
+  <si>
+    <t>CS102B-L2</t>
+  </si>
+  <si>
+    <t>CS101A-L1</t>
+  </si>
+  <si>
+    <t>CS101A-L2</t>
+  </si>
+  <si>
+    <t>CS101B-L</t>
+  </si>
+  <si>
+    <t>CS103A-L</t>
+  </si>
+  <si>
+    <t>CS103B-L</t>
+  </si>
+  <si>
+    <t>NS104A-L</t>
+  </si>
+  <si>
+    <t>NS104B-L</t>
+  </si>
+  <si>
+    <t>CS104A-L</t>
+  </si>
+  <si>
+    <t>CS104B-L</t>
   </si>
 </sst>
 </file>
@@ -822,9 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -836,13 +834,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -850,13 +848,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -864,13 +862,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -878,13 +876,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -892,13 +890,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -906,69 +904,69 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -976,27 +974,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1004,13 +1002,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1018,13 +1016,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1032,13 +1030,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1046,13 +1044,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1060,590 +1058,590 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
         <v>73</v>
       </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
-      </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
       </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
-      </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D41" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D46" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" t="s">
         <v>108</v>
-      </c>
-      <c r="C52" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D55" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" t="s">
         <v>115</v>
-      </c>
-      <c r="D57" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Loader for ClassRoom
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="142">
   <si>
     <t>Teacher Name</t>
   </si>
@@ -428,6 +428,18 @@
   </si>
   <si>
     <t>CS104B-L</t>
+  </si>
+  <si>
+    <t>HU104A</t>
+  </si>
+  <si>
+    <t>Functional English</t>
+  </si>
+  <si>
+    <t>Sharmeen</t>
+  </si>
+  <si>
+    <t>HU104B</t>
   </si>
 </sst>
 </file>
@@ -820,9 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -876,69 +890,69 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -946,13 +960,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -960,69 +974,69 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1030,150 +1044,150 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
         <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
         <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
         <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>73</v>
@@ -1184,10 +1198,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
         <v>74</v>
@@ -1198,38 +1212,38 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
         <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>73</v>
@@ -1240,10 +1254,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>74</v>
@@ -1254,393 +1268,421 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
         <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
         <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
         <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
         <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
         <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
         <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
         <v>75</v>
       </c>
       <c r="D40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
         <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
         <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
         <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>80</v>
       </c>
       <c r="D46" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
         <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D48" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D49" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
         <v>81</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
         <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C52" t="s">
         <v>81</v>
       </c>
       <c r="D52" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
         <v>81</v>
       </c>
       <c r="D53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
         <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D55" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
         <v>102</v>
       </c>
       <c r="D57" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
         <v>102</v>
       </c>
       <c r="D58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>